<commit_message>
Mise à jour outils
</commit_message>
<xml_diff>
--- a/tools/fiche_impacts_developpements.xlsx
+++ b/tools/fiche_impacts_developpements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\inside\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FC4A8C-41AB-490D-98F7-C4FD142E4743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CFCD68-9AA4-420D-AA4F-490C7461A1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D2EF4CBC-F83C-4668-9017-B1316576DC81}"/>
   </bookViews>
@@ -415,9 +415,6 @@
     <t>Doit-on mettre à jour le kit d’installation ?</t>
   </si>
   <si>
-    <t>Le kit d’installation se trouve à la racine du dossier source (install.rar) et doit être mis à jour dès qu’il y a des modifications de la structure de la base de données (script inside.sql), parfois de son contenu (par exemple de nouvelles alertes) ou qu’il y a de nouvelles images à fournir aux développeurs pour les succès.</t>
-  </si>
-  <si>
     <t>Est-ce que toutes les tables modifiées l’ont été sur la version en ligne ?</t>
   </si>
   <si>
@@ -789,6 +786,9 @@
   </si>
   <si>
     <t>Impact (Oui – Non)</t>
+  </si>
+  <si>
+    <t>Le kit d’installation se trouve à la racine du dossier source (install.rar) et doit être mis à jour dès qu’il y a des modifications de la structure de la base de données (script inside.sql), parfois de son contenu (par exemple de nouvelles alertes ou de nouveaux succès) ou qu’il y a de nouvelles images à fournir aux développeurs pour les succès.</t>
   </si>
 </sst>
 </file>
@@ -1011,53 +1011,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1092,7 +1050,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>740025</xdr:colOff>
+      <xdr:colOff>743835</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>113157</xdr:rowOff>
     </xdr:to>
@@ -1435,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F16EF5E-4CBF-4A5F-BD98-678C676B6231}">
   <dimension ref="A2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1474,7 +1432,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>5</v>
@@ -1534,7 +1492,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1542,10 +1500,10 @@
     <row r="12" spans="1:5" ht="159" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1569,7 +1527,7 @@
         <v>20</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1602,7 +1560,7 @@
         <v>25</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1650,7 +1608,7 @@
         <v>34</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1685,7 +1643,7 @@
         <v>40</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1709,7 +1667,7 @@
         <v>44</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -1735,18 +1693,18 @@
         <v>49</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="58.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -1754,36 +1712,36 @@
     <row r="30" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -1796,10 +1754,10 @@
     <mergeCell ref="A4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E32">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Correction style boutons web & mise à jour fiche impacts
</commit_message>
<xml_diff>
--- a/tools/fiche_impacts_developpements.xlsx
+++ b/tools/fiche_impacts_developpements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\inside\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CFCD68-9AA4-420D-AA4F-490C7461A1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8C9B1F-7D4A-413D-841D-72A16D2FC5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D2EF4CBC-F83C-4668-9017-B1316576DC81}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Fiche impacts de développements</t>
   </si>
@@ -789,6 +789,12 @@
   </si>
   <si>
     <t>Le kit d’installation se trouve à la racine du dossier source (install.rar) et doit être mis à jour dès qu’il y a des modifications de la structure de la base de données (script inside.sql), parfois de son contenu (par exemple de nouvelles alertes ou de nouveaux succès) ou qu’il y a de nouvelles images à fournir aux développeurs pour les succès.</t>
+  </si>
+  <si>
+    <t>Est-il prévu de conserver les saisies utilisateurs lorsqu'un alerte est déclenchée ?</t>
+  </si>
+  <si>
+    <t>Si oui, prévoir de sauvegarder les données en $_SESSION.</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1017,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1023,6 +1036,13 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1391,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F16EF5E-4CBF-4A5F-BD98-678C676B6231}">
-  <dimension ref="A2:E33"/>
+  <dimension ref="A2:E34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1463,163 +1483,163 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>62</v>
+    <row r="11" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="159" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>59</v>
+        <v>16</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>17</v>
-      </c>
+    <row r="13" spans="1:5" ht="159" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
       <c r="B13" s="8" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="B14" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>22</v>
+    <row r="15" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="58.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>24</v>
+    <row r="16" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
-      <c r="B17" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>63</v>
+    <row r="17" spans="1:5" ht="58.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>28</v>
+    <row r="18" spans="1:5" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="11"/>
+      <c r="B18" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
+    <row r="19" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="B19" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
-      <c r="B21" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>64</v>
+    <row r="21" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>36</v>
+    <row r="22" spans="1:5" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="11"/>
+      <c r="B22" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1627,145 +1647,164 @@
     <row r="23" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>65</v>
+    <row r="24" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>42</v>
+    <row r="25" spans="1:5" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>66</v>
+    <row r="26" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>47</v>
+    <row r="27" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>67</v>
+    <row r="28" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="58.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>69</v>
+    <row r="29" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="58.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>53</v>
-      </c>
+    <row r="31" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="3"/>
       <c r="B31" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:E32">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+  <conditionalFormatting sqref="D7:E7 D9:E33">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:E8">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Non"</formula>
+      <formula>"Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E32" xr:uid="{A853E13E-3CCC-4A59-BF9A-DABDAA5A6426}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E33" xr:uid="{A853E13E-3CCC-4A59-BF9A-DABDAA5A6426}">
       <formula1>"Oui,Non,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D32" xr:uid="{A4A0FD31-5BD8-4AF6-8CE1-BA0E09B5E07D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D33" xr:uid="{A4A0FD31-5BD8-4AF6-8CE1-BA0E09B5E07D}">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>